<commit_message>
export file in different CRS
</commit_message>
<xml_diff>
--- a/assets/cn.xlsx
+++ b/assets/cn.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E235"/>
+  <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,10 +489,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>58.35000228881836</v>
+        <v>6495990.83146653</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>42005</v>
@@ -501,13 +501,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>42005</v>
@@ -516,13 +516,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>42005</v>
@@ -537,7 +537,7 @@
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="n">
-        <v>36.75</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>42005</v>
@@ -546,13 +546,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>42005</v>
@@ -567,7 +567,7 @@
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>42005</v>
@@ -576,13 +576,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>42005</v>
@@ -591,13 +591,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>42005</v>
@@ -606,13 +606,13 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="n">
-        <v>36.25</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>42005</v>
@@ -621,13 +621,13 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>42005</v>
@@ -642,7 +642,7 @@
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>42005</v>
@@ -651,13 +651,13 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>42005</v>
@@ -666,13 +666,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>42005</v>
@@ -681,15 +681,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>58.45000839233398</v>
-      </c>
+      <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>42005</v>
@@ -698,13 +696,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>42005</v>
@@ -717,9 +715,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n"/>
+      <c r="A17" s="1" t="n">
+        <v>6508119.338340166</v>
+      </c>
       <c r="B17" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>42005</v>
@@ -728,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="n">
-        <v>36.75</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>42005</v>
@@ -743,13 +743,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>42005</v>
@@ -758,13 +758,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>42005</v>
@@ -773,13 +773,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>42005</v>
@@ -788,13 +788,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>42005</v>
@@ -809,7 +809,7 @@
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="n">
-        <v>36.25</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>42005</v>
@@ -818,13 +818,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>42005</v>
@@ -839,7 +839,7 @@
     <row r="25">
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>42005</v>
@@ -848,13 +848,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>42005</v>
@@ -863,13 +863,13 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>42005</v>
@@ -882,11 +882,9 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>58.54999923706055</v>
-      </c>
+      <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>42005</v>
@@ -895,13 +893,13 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>42005</v>
@@ -910,13 +908,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>42005</v>
@@ -925,13 +923,13 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="n">
-        <v>36.75</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>42005</v>
@@ -940,13 +938,15 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n"/>
+      <c r="A32" s="1" t="n">
+        <v>6520247.845213803</v>
+      </c>
       <c r="B32" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>42005</v>
@@ -955,13 +955,13 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>42005</v>
@@ -976,7 +976,7 @@
     <row r="34">
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>42005</v>
@@ -985,13 +985,13 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>42005</v>
@@ -1000,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="n">
-        <v>36.25</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>42005</v>
@@ -1015,13 +1015,13 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>42005</v>
@@ -1030,13 +1030,13 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>42005</v>
@@ -1045,13 +1045,13 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>42005</v>
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>42005</v>
@@ -1075,15 +1075,13 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>58.65000534057617</v>
-      </c>
+      <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>42005</v>
@@ -1098,7 +1096,7 @@
     <row r="42">
       <c r="A42" s="1" t="n"/>
       <c r="B42" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>42005</v>
@@ -1107,13 +1105,13 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
       <c r="B43" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>42005</v>
@@ -1122,13 +1120,13 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
       <c r="B44" s="1" t="n">
-        <v>36.75</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>42005</v>
@@ -1137,13 +1135,13 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
       <c r="B45" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>42005</v>
@@ -1152,13 +1150,13 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
       <c r="B46" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>42005</v>
@@ -1167,13 +1165,15 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n"/>
+      <c r="A47" s="1" t="n">
+        <v>6532376.35208744</v>
+      </c>
       <c r="B47" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>42005</v>
@@ -1182,13 +1182,13 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
       <c r="B48" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>42005</v>
@@ -1203,7 +1203,7 @@
     <row r="49">
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="n">
-        <v>36.25</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>42005</v>
@@ -1212,13 +1212,13 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
       <c r="B50" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>42005</v>
@@ -1227,13 +1227,13 @@
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n"/>
       <c r="B51" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>42005</v>
@@ -1242,13 +1242,13 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
       <c r="B52" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>42005</v>
@@ -1257,13 +1257,13 @@
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
       <c r="B53" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>42005</v>
@@ -1276,11 +1276,9 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>58.74999618530273</v>
-      </c>
+      <c r="A54" s="1" t="n"/>
       <c r="B54" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C54" s="2" t="n">
         <v>42005</v>
@@ -1289,13 +1287,13 @@
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
       <c r="B55" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C55" s="2" t="n">
         <v>42005</v>
@@ -1304,13 +1302,13 @@
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
       <c r="B56" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C56" s="2" t="n">
         <v>42005</v>
@@ -1325,7 +1323,7 @@
     <row r="57">
       <c r="A57" s="1" t="n"/>
       <c r="B57" s="1" t="n">
-        <v>36.75</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C57" s="2" t="n">
         <v>42005</v>
@@ -1334,13 +1332,13 @@
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n"/>
       <c r="B58" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>42005</v>
@@ -1349,13 +1347,13 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
       <c r="B59" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C59" s="2" t="n">
         <v>42005</v>
@@ -1370,7 +1368,7 @@
     <row r="60">
       <c r="A60" s="1" t="n"/>
       <c r="B60" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>42005</v>
@@ -1385,7 +1383,7 @@
     <row r="61">
       <c r="A61" s="1" t="n"/>
       <c r="B61" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>42005</v>
@@ -1394,13 +1392,15 @@
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n"/>
+      <c r="A62" s="1" t="n">
+        <v>6544504.858961076</v>
+      </c>
       <c r="B62" s="1" t="n">
-        <v>36.25</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>42005</v>
@@ -1409,13 +1409,13 @@
         <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
       <c r="B63" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>42005</v>
@@ -1424,13 +1424,13 @@
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
       <c r="B64" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>42005</v>
@@ -1439,13 +1439,13 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
       <c r="B65" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>42005</v>
@@ -1460,7 +1460,7 @@
     <row r="66">
       <c r="A66" s="1" t="n"/>
       <c r="B66" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C66" s="2" t="n">
         <v>42005</v>
@@ -1469,15 +1469,13 @@
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>58.85000228881836</v>
-      </c>
+      <c r="A67" s="1" t="n"/>
       <c r="B67" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>42005</v>
@@ -1486,13 +1484,13 @@
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
       <c r="B68" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>42005</v>
@@ -1501,13 +1499,13 @@
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
       <c r="B69" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>42005</v>
@@ -1516,13 +1514,13 @@
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
       <c r="B70" s="1" t="n">
-        <v>36.75</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>42005</v>
@@ -1531,13 +1529,13 @@
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
       <c r="B71" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C71" s="2" t="n">
         <v>42005</v>
@@ -1546,13 +1544,13 @@
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
       <c r="B72" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C72" s="2" t="n">
         <v>42005</v>
@@ -1561,13 +1559,13 @@
         <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
       <c r="B73" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C73" s="2" t="n">
         <v>42005</v>
@@ -1576,13 +1574,13 @@
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
       <c r="B74" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C74" s="2" t="n">
         <v>42005</v>
@@ -1591,13 +1589,13 @@
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
       <c r="B75" s="1" t="n">
-        <v>36.25</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C75" s="2" t="n">
         <v>42005</v>
@@ -1606,13 +1604,13 @@
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
       <c r="B76" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>42005</v>
@@ -1621,13 +1619,15 @@
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n"/>
+      <c r="A77" s="1" t="n">
+        <v>6556633.365834713</v>
+      </c>
       <c r="B77" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C77" s="2" t="n">
         <v>42005</v>
@@ -1636,13 +1636,13 @@
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
       <c r="B78" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C78" s="2" t="n">
         <v>42005</v>
@@ -1651,13 +1651,13 @@
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n"/>
       <c r="B79" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C79" s="2" t="n">
         <v>42005</v>
@@ -1666,15 +1666,13 @@
         <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>58.95000839233398</v>
-      </c>
+      <c r="A80" s="1" t="n"/>
       <c r="B80" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C80" s="2" t="n">
         <v>42005</v>
@@ -1683,13 +1681,13 @@
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
       <c r="B81" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C81" s="2" t="n">
         <v>42005</v>
@@ -1698,13 +1696,13 @@
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
       <c r="B82" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C82" s="2" t="n">
         <v>42005</v>
@@ -1713,13 +1711,13 @@
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
       <c r="B83" s="1" t="n">
-        <v>36.75</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C83" s="2" t="n">
         <v>42005</v>
@@ -1728,13 +1726,13 @@
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
       <c r="B84" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C84" s="2" t="n">
         <v>42005</v>
@@ -1743,13 +1741,13 @@
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
       <c r="B85" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C85" s="2" t="n">
         <v>42005</v>
@@ -1758,13 +1756,13 @@
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
       <c r="B86" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C86" s="2" t="n">
         <v>42005</v>
@@ -1773,13 +1771,13 @@
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
       <c r="B87" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C87" s="2" t="n">
         <v>42005</v>
@@ -1788,13 +1786,13 @@
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
       <c r="B88" s="1" t="n">
-        <v>36.25</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C88" s="2" t="n">
         <v>42005</v>
@@ -1803,13 +1801,13 @@
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
       <c r="B89" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C89" s="2" t="n">
         <v>42005</v>
@@ -1818,13 +1816,13 @@
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
       <c r="B90" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>42005</v>
@@ -1833,13 +1831,13 @@
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
       <c r="B91" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C91" s="2" t="n">
         <v>42005</v>
@@ -1848,13 +1846,15 @@
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n"/>
+      <c r="A92" s="1" t="n">
+        <v>6568761.87270835</v>
+      </c>
       <c r="B92" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C92" s="2" t="n">
         <v>42005</v>
@@ -1863,15 +1863,13 @@
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>59.04999923706055</v>
-      </c>
+      <c r="A93" s="1" t="n"/>
       <c r="B93" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C93" s="2" t="n">
         <v>42005</v>
@@ -1880,13 +1878,13 @@
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
       <c r="B94" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C94" s="2" t="n">
         <v>42005</v>
@@ -1895,13 +1893,13 @@
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
       <c r="B95" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C95" s="2" t="n">
         <v>42005</v>
@@ -1910,13 +1908,13 @@
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
       <c r="B96" s="1" t="n">
-        <v>36.75</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C96" s="2" t="n">
         <v>42005</v>
@@ -1925,13 +1923,13 @@
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
       <c r="B97" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C97" s="2" t="n">
         <v>42005</v>
@@ -1946,7 +1944,7 @@
     <row r="98">
       <c r="A98" s="1" t="n"/>
       <c r="B98" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C98" s="2" t="n">
         <v>42005</v>
@@ -1961,7 +1959,7 @@
     <row r="99">
       <c r="A99" s="1" t="n"/>
       <c r="B99" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C99" s="2" t="n">
         <v>42005</v>
@@ -1976,7 +1974,7 @@
     <row r="100">
       <c r="A100" s="1" t="n"/>
       <c r="B100" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C100" s="2" t="n">
         <v>42005</v>
@@ -1984,12 +1982,14 @@
       <c r="D100" t="n">
         <v>0</v>
       </c>
-      <c r="E100" t="inlineStr"/>
+      <c r="E100" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
       <c r="B101" s="1" t="n">
-        <v>36.25</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C101" s="2" t="n">
         <v>42005</v>
@@ -2004,7 +2004,7 @@
     <row r="102">
       <c r="A102" s="1" t="n"/>
       <c r="B102" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C102" s="2" t="n">
         <v>42005</v>
@@ -2013,13 +2013,13 @@
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
       <c r="B103" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C103" s="2" t="n">
         <v>42005</v>
@@ -2034,7 +2034,7 @@
     <row r="104">
       <c r="A104" s="1" t="n"/>
       <c r="B104" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C104" s="2" t="n">
         <v>42005</v>
@@ -2043,13 +2043,13 @@
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
       <c r="B105" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C105" s="2" t="n">
         <v>42005</v>
@@ -2058,15 +2058,13 @@
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>59.15000534057617</v>
-      </c>
+      <c r="A106" s="1" t="n"/>
       <c r="B106" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C106" s="2" t="n">
         <v>42005</v>
@@ -2075,13 +2073,15 @@
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n"/>
+      <c r="A107" s="1" t="n">
+        <v>6580890.379581987</v>
+      </c>
       <c r="B107" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C107" s="2" t="n">
         <v>42005</v>
@@ -2090,13 +2090,13 @@
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n"/>
       <c r="B108" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C108" s="2" t="n">
         <v>42005</v>
@@ -2111,7 +2111,7 @@
     <row r="109">
       <c r="A109" s="1" t="n"/>
       <c r="B109" s="1" t="n">
-        <v>36.75</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C109" s="2" t="n">
         <v>42005</v>
@@ -2120,13 +2120,13 @@
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n"/>
       <c r="B110" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C110" s="2" t="n">
         <v>42005</v>
@@ -2135,13 +2135,13 @@
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n"/>
       <c r="B111" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C111" s="2" t="n">
         <v>42005</v>
@@ -2150,13 +2150,13 @@
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n"/>
       <c r="B112" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C112" s="2" t="n">
         <v>42005</v>
@@ -2165,13 +2165,13 @@
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n"/>
       <c r="B113" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C113" s="2" t="n">
         <v>42005</v>
@@ -2180,13 +2180,13 @@
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n"/>
       <c r="B114" s="1" t="n">
-        <v>36.25</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C114" s="2" t="n">
         <v>42005</v>
@@ -2195,13 +2195,13 @@
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n"/>
       <c r="B115" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C115" s="2" t="n">
         <v>42005</v>
@@ -2216,7 +2216,7 @@
     <row r="116">
       <c r="A116" s="1" t="n"/>
       <c r="B116" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C116" s="2" t="n">
         <v>42005</v>
@@ -2225,13 +2225,13 @@
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n"/>
       <c r="B117" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C117" s="2" t="n">
         <v>42005</v>
@@ -2240,13 +2240,13 @@
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n"/>
       <c r="B118" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C118" s="2" t="n">
         <v>42005</v>
@@ -2259,11 +2259,9 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>59.24999618530273</v>
-      </c>
+      <c r="A119" s="1" t="n"/>
       <c r="B119" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C119" s="2" t="n">
         <v>42005</v>
@@ -2272,13 +2270,13 @@
         <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n"/>
       <c r="B120" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C120" s="2" t="n">
         <v>42005</v>
@@ -2287,13 +2285,13 @@
         <v>0</v>
       </c>
       <c r="E120" t="n">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n"/>
       <c r="B121" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C121" s="2" t="n">
         <v>42005</v>
@@ -2302,13 +2300,15 @@
         <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n"/>
+      <c r="A122" s="1" t="n">
+        <v>6593018.886455623</v>
+      </c>
       <c r="B122" s="1" t="n">
-        <v>36.75</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C122" s="2" t="n">
         <v>42005</v>
@@ -2323,7 +2323,7 @@
     <row r="123">
       <c r="A123" s="1" t="n"/>
       <c r="B123" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C123" s="2" t="n">
         <v>42005</v>
@@ -2332,13 +2332,13 @@
         <v>0</v>
       </c>
       <c r="E123" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n"/>
       <c r="B124" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C124" s="2" t="n">
         <v>42005</v>
@@ -2347,13 +2347,13 @@
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n"/>
       <c r="B125" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C125" s="2" t="n">
         <v>42005</v>
@@ -2362,13 +2362,13 @@
         <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n"/>
       <c r="B126" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C126" s="2" t="n">
         <v>42005</v>
@@ -2377,13 +2377,13 @@
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n"/>
       <c r="B127" s="1" t="n">
-        <v>36.25</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C127" s="2" t="n">
         <v>42005</v>
@@ -2392,13 +2392,13 @@
         <v>0</v>
       </c>
       <c r="E127" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n"/>
       <c r="B128" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C128" s="2" t="n">
         <v>42005</v>
@@ -2407,13 +2407,13 @@
         <v>0</v>
       </c>
       <c r="E128" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n"/>
       <c r="B129" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C129" s="2" t="n">
         <v>42005</v>
@@ -2422,13 +2422,13 @@
         <v>0</v>
       </c>
       <c r="E129" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n"/>
       <c r="B130" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C130" s="2" t="n">
         <v>42005</v>
@@ -2437,13 +2437,13 @@
         <v>0</v>
       </c>
       <c r="E130" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n"/>
       <c r="B131" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C131" s="2" t="n">
         <v>42005</v>
@@ -2452,15 +2452,13 @@
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>59.35000228881836</v>
-      </c>
+      <c r="A132" s="1" t="n"/>
       <c r="B132" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C132" s="2" t="n">
         <v>42005</v>
@@ -2469,13 +2467,13 @@
         <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n"/>
       <c r="B133" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C133" s="2" t="n">
         <v>42005</v>
@@ -2484,13 +2482,13 @@
         <v>0</v>
       </c>
       <c r="E133" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n"/>
       <c r="B134" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C134" s="2" t="n">
         <v>42005</v>
@@ -2505,7 +2503,7 @@
     <row r="135">
       <c r="A135" s="1" t="n"/>
       <c r="B135" s="1" t="n">
-        <v>36.75</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C135" s="2" t="n">
         <v>42005</v>
@@ -2514,13 +2512,13 @@
         <v>0</v>
       </c>
       <c r="E135" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n"/>
       <c r="B136" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C136" s="2" t="n">
         <v>42005</v>
@@ -2529,13 +2527,15 @@
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="n"/>
+      <c r="A137" s="1" t="n">
+        <v>6605147.393329261</v>
+      </c>
       <c r="B137" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C137" s="2" t="n">
         <v>42005</v>
@@ -2544,13 +2544,13 @@
         <v>0</v>
       </c>
       <c r="E137" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n"/>
       <c r="B138" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C138" s="2" t="n">
         <v>42005</v>
@@ -2559,13 +2559,13 @@
         <v>0</v>
       </c>
       <c r="E138" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n"/>
       <c r="B139" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C139" s="2" t="n">
         <v>42005</v>
@@ -2574,13 +2574,13 @@
         <v>0</v>
       </c>
       <c r="E139" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n"/>
       <c r="B140" s="1" t="n">
-        <v>36.25</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C140" s="2" t="n">
         <v>42005</v>
@@ -2589,13 +2589,13 @@
         <v>0</v>
       </c>
       <c r="E140" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n"/>
       <c r="B141" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C141" s="2" t="n">
         <v>42005</v>
@@ -2604,13 +2604,13 @@
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n"/>
       <c r="B142" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C142" s="2" t="n">
         <v>42005</v>
@@ -2619,13 +2619,13 @@
         <v>0</v>
       </c>
       <c r="E142" t="n">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n"/>
       <c r="B143" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C143" s="2" t="n">
         <v>42005</v>
@@ -2634,13 +2634,13 @@
         <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n"/>
       <c r="B144" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C144" s="2" t="n">
         <v>42005</v>
@@ -2649,15 +2649,13 @@
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>59.45000839233398</v>
-      </c>
+      <c r="A145" s="1" t="n"/>
       <c r="B145" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C145" s="2" t="n">
         <v>42005</v>
@@ -2666,13 +2664,13 @@
         <v>0</v>
       </c>
       <c r="E145" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n"/>
       <c r="B146" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C146" s="2" t="n">
         <v>42005</v>
@@ -2681,13 +2679,13 @@
         <v>0</v>
       </c>
       <c r="E146" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n"/>
       <c r="B147" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C147" s="2" t="n">
         <v>42005</v>
@@ -2696,13 +2694,13 @@
         <v>0</v>
       </c>
       <c r="E147" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n"/>
       <c r="B148" s="1" t="n">
-        <v>36.75</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C148" s="2" t="n">
         <v>42005</v>
@@ -2711,13 +2709,13 @@
         <v>0</v>
       </c>
       <c r="E148" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n"/>
       <c r="B149" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C149" s="2" t="n">
         <v>42005</v>
@@ -2726,13 +2724,13 @@
         <v>0</v>
       </c>
       <c r="E149" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n"/>
       <c r="B150" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C150" s="2" t="n">
         <v>42005</v>
@@ -2741,13 +2739,13 @@
         <v>0</v>
       </c>
       <c r="E150" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n"/>
       <c r="B151" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C151" s="2" t="n">
         <v>42005</v>
@@ -2756,13 +2754,15 @@
         <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="1" t="n"/>
+      <c r="A152" s="1" t="n">
+        <v>6617275.900202897</v>
+      </c>
       <c r="B152" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C152" s="2" t="n">
         <v>42005</v>
@@ -2771,13 +2771,13 @@
         <v>0</v>
       </c>
       <c r="E152" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n"/>
       <c r="B153" s="1" t="n">
-        <v>36.25</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C153" s="2" t="n">
         <v>42005</v>
@@ -2786,13 +2786,13 @@
         <v>0</v>
       </c>
       <c r="E153" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n"/>
       <c r="B154" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C154" s="2" t="n">
         <v>42005</v>
@@ -2801,13 +2801,13 @@
         <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n"/>
       <c r="B155" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C155" s="2" t="n">
         <v>42005</v>
@@ -2816,13 +2816,13 @@
         <v>0</v>
       </c>
       <c r="E155" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n"/>
       <c r="B156" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C156" s="2" t="n">
         <v>42005</v>
@@ -2831,13 +2831,13 @@
         <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n"/>
       <c r="B157" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C157" s="2" t="n">
         <v>42005</v>
@@ -2846,15 +2846,13 @@
         <v>0</v>
       </c>
       <c r="E157" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="1" t="n">
-        <v>59.54999923706055</v>
-      </c>
+      <c r="A158" s="1" t="n"/>
       <c r="B158" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C158" s="2" t="n">
         <v>42005</v>
@@ -2863,13 +2861,13 @@
         <v>0</v>
       </c>
       <c r="E158" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n"/>
       <c r="B159" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C159" s="2" t="n">
         <v>42005</v>
@@ -2878,13 +2876,13 @@
         <v>0</v>
       </c>
       <c r="E159" t="n">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n"/>
       <c r="B160" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C160" s="2" t="n">
         <v>42005</v>
@@ -2899,7 +2897,7 @@
     <row r="161">
       <c r="A161" s="1" t="n"/>
       <c r="B161" s="1" t="n">
-        <v>36.75</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C161" s="2" t="n">
         <v>42005</v>
@@ -2914,7 +2912,7 @@
     <row r="162">
       <c r="A162" s="1" t="n"/>
       <c r="B162" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C162" s="2" t="n">
         <v>42005</v>
@@ -2923,13 +2921,13 @@
         <v>0</v>
       </c>
       <c r="E162" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n"/>
       <c r="B163" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C163" s="2" t="n">
         <v>42005</v>
@@ -2938,13 +2936,13 @@
         <v>0</v>
       </c>
       <c r="E163" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n"/>
       <c r="B164" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C164" s="2" t="n">
         <v>42005</v>
@@ -2953,13 +2951,13 @@
         <v>0</v>
       </c>
       <c r="E164" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n"/>
       <c r="B165" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C165" s="2" t="n">
         <v>42005</v>
@@ -2974,7 +2972,7 @@
     <row r="166">
       <c r="A166" s="1" t="n"/>
       <c r="B166" s="1" t="n">
-        <v>36.25</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C166" s="2" t="n">
         <v>42005</v>
@@ -2983,13 +2981,15 @@
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="1" t="n"/>
+      <c r="A167" s="1" t="n">
+        <v>6629404.407076534</v>
+      </c>
       <c r="B167" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C167" s="2" t="n">
         <v>42005</v>
@@ -2998,13 +2998,13 @@
         <v>0</v>
       </c>
       <c r="E167" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n"/>
       <c r="B168" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C168" s="2" t="n">
         <v>42005</v>
@@ -3013,13 +3013,13 @@
         <v>0</v>
       </c>
       <c r="E168" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n"/>
       <c r="B169" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C169" s="2" t="n">
         <v>42005</v>
@@ -3034,7 +3034,7 @@
     <row r="170">
       <c r="A170" s="1" t="n"/>
       <c r="B170" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C170" s="2" t="n">
         <v>42005</v>
@@ -3043,15 +3043,13 @@
         <v>0</v>
       </c>
       <c r="E170" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="1" t="n">
-        <v>59.65000534057617</v>
-      </c>
+      <c r="A171" s="1" t="n"/>
       <c r="B171" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C171" s="2" t="n">
         <v>42005</v>
@@ -3060,13 +3058,13 @@
         <v>0</v>
       </c>
       <c r="E171" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n"/>
       <c r="B172" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C172" s="2" t="n">
         <v>42005</v>
@@ -3075,13 +3073,13 @@
         <v>0</v>
       </c>
       <c r="E172" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n"/>
       <c r="B173" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C173" s="2" t="n">
         <v>42005</v>
@@ -3090,13 +3088,13 @@
         <v>0</v>
       </c>
       <c r="E173" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n"/>
       <c r="B174" s="1" t="n">
-        <v>36.75</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C174" s="2" t="n">
         <v>42005</v>
@@ -3111,7 +3109,7 @@
     <row r="175">
       <c r="A175" s="1" t="n"/>
       <c r="B175" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C175" s="2" t="n">
         <v>42005</v>
@@ -3126,7 +3124,7 @@
     <row r="176">
       <c r="A176" s="1" t="n"/>
       <c r="B176" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C176" s="2" t="n">
         <v>42005</v>
@@ -3135,13 +3133,13 @@
         <v>0</v>
       </c>
       <c r="E176" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n"/>
       <c r="B177" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C177" s="2" t="n">
         <v>42005</v>
@@ -3150,13 +3148,13 @@
         <v>0</v>
       </c>
       <c r="E177" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n"/>
       <c r="B178" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C178" s="2" t="n">
         <v>42005</v>
@@ -3165,13 +3163,13 @@
         <v>0</v>
       </c>
       <c r="E178" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n"/>
       <c r="B179" s="1" t="n">
-        <v>36.25</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C179" s="2" t="n">
         <v>42005</v>
@@ -3180,13 +3178,13 @@
         <v>0</v>
       </c>
       <c r="E179" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n"/>
       <c r="B180" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C180" s="2" t="n">
         <v>42005</v>
@@ -3195,13 +3193,13 @@
         <v>0</v>
       </c>
       <c r="E180" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n"/>
       <c r="B181" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C181" s="2" t="n">
         <v>42005</v>
@@ -3210,13 +3208,15 @@
         <v>0</v>
       </c>
       <c r="E181" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="1" t="n"/>
+      <c r="A182" s="1" t="n">
+        <v>6641532.91395017</v>
+      </c>
       <c r="B182" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C182" s="2" t="n">
         <v>42005</v>
@@ -3225,13 +3225,13 @@
         <v>0</v>
       </c>
       <c r="E182" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n"/>
       <c r="B183" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C183" s="2" t="n">
         <v>42005</v>
@@ -3240,15 +3240,13 @@
         <v>0</v>
       </c>
       <c r="E183" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="1" t="n">
-        <v>59.74999618530273</v>
-      </c>
+      <c r="A184" s="1" t="n"/>
       <c r="B184" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C184" s="2" t="n">
         <v>42005</v>
@@ -3263,7 +3261,7 @@
     <row r="185">
       <c r="A185" s="1" t="n"/>
       <c r="B185" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C185" s="2" t="n">
         <v>42005</v>
@@ -3272,13 +3270,13 @@
         <v>0</v>
       </c>
       <c r="E185" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n"/>
       <c r="B186" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C186" s="2" t="n">
         <v>42005</v>
@@ -3287,13 +3285,13 @@
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n"/>
       <c r="B187" s="1" t="n">
-        <v>36.75</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C187" s="2" t="n">
         <v>42005</v>
@@ -3308,7 +3306,7 @@
     <row r="188">
       <c r="A188" s="1" t="n"/>
       <c r="B188" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C188" s="2" t="n">
         <v>42005</v>
@@ -3317,13 +3315,13 @@
         <v>0</v>
       </c>
       <c r="E188" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n"/>
       <c r="B189" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C189" s="2" t="n">
         <v>42005</v>
@@ -3338,7 +3336,7 @@
     <row r="190">
       <c r="A190" s="1" t="n"/>
       <c r="B190" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C190" s="2" t="n">
         <v>42005</v>
@@ -3347,13 +3345,13 @@
         <v>0</v>
       </c>
       <c r="E190" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n"/>
       <c r="B191" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C191" s="2" t="n">
         <v>42005</v>
@@ -3362,13 +3360,13 @@
         <v>0</v>
       </c>
       <c r="E191" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n"/>
       <c r="B192" s="1" t="n">
-        <v>36.25</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C192" s="2" t="n">
         <v>42005</v>
@@ -3377,13 +3375,13 @@
         <v>0</v>
       </c>
       <c r="E192" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n"/>
       <c r="B193" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C193" s="2" t="n">
         <v>42005</v>
@@ -3392,13 +3390,13 @@
         <v>0</v>
       </c>
       <c r="E193" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n"/>
       <c r="B194" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C194" s="2" t="n">
         <v>42005</v>
@@ -3407,13 +3405,13 @@
         <v>0</v>
       </c>
       <c r="E194" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n"/>
       <c r="B195" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C195" s="2" t="n">
         <v>42005</v>
@@ -3422,13 +3420,13 @@
         <v>0</v>
       </c>
       <c r="E195" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n"/>
       <c r="B196" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C196" s="2" t="n">
         <v>42005</v>
@@ -3437,15 +3435,15 @@
         <v>0</v>
       </c>
       <c r="E196" t="n">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>59.85000228881836</v>
+        <v>6653661.420823808</v>
       </c>
       <c r="B197" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C197" s="2" t="n">
         <v>42005</v>
@@ -3454,13 +3452,13 @@
         <v>0</v>
       </c>
       <c r="E197" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n"/>
       <c r="B198" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C198" s="2" t="n">
         <v>42005</v>
@@ -3469,13 +3467,13 @@
         <v>0</v>
       </c>
       <c r="E198" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n"/>
       <c r="B199" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C199" s="2" t="n">
         <v>42005</v>
@@ -3484,13 +3482,13 @@
         <v>0</v>
       </c>
       <c r="E199" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n"/>
       <c r="B200" s="1" t="n">
-        <v>36.75</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C200" s="2" t="n">
         <v>42005</v>
@@ -3505,7 +3503,7 @@
     <row r="201">
       <c r="A201" s="1" t="n"/>
       <c r="B201" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C201" s="2" t="n">
         <v>42005</v>
@@ -3514,13 +3512,13 @@
         <v>0</v>
       </c>
       <c r="E201" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n"/>
       <c r="B202" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C202" s="2" t="n">
         <v>42005</v>
@@ -3529,13 +3527,13 @@
         <v>0</v>
       </c>
       <c r="E202" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n"/>
       <c r="B203" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C203" s="2" t="n">
         <v>42005</v>
@@ -3550,7 +3548,7 @@
     <row r="204">
       <c r="A204" s="1" t="n"/>
       <c r="B204" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C204" s="2" t="n">
         <v>42005</v>
@@ -3565,7 +3563,7 @@
     <row r="205">
       <c r="A205" s="1" t="n"/>
       <c r="B205" s="1" t="n">
-        <v>36.25</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C205" s="2" t="n">
         <v>42005</v>
@@ -3574,13 +3572,13 @@
         <v>0</v>
       </c>
       <c r="E205" t="n">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n"/>
       <c r="B206" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C206" s="2" t="n">
         <v>42005</v>
@@ -3595,7 +3593,7 @@
     <row r="207">
       <c r="A207" s="1" t="n"/>
       <c r="B207" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C207" s="2" t="n">
         <v>42005</v>
@@ -3610,7 +3608,7 @@
     <row r="208">
       <c r="A208" s="1" t="n"/>
       <c r="B208" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C208" s="2" t="n">
         <v>42005</v>
@@ -3619,13 +3617,13 @@
         <v>0</v>
       </c>
       <c r="E208" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n"/>
       <c r="B209" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C209" s="2" t="n">
         <v>42005</v>
@@ -3634,15 +3632,13 @@
         <v>0</v>
       </c>
       <c r="E209" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="1" t="n">
-        <v>59.95000839233398</v>
-      </c>
+      <c r="A210" s="1" t="n"/>
       <c r="B210" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C210" s="2" t="n">
         <v>42005</v>
@@ -3651,13 +3647,13 @@
         <v>0</v>
       </c>
       <c r="E210" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n"/>
       <c r="B211" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C211" s="2" t="n">
         <v>42005</v>
@@ -3666,13 +3662,15 @@
         <v>0</v>
       </c>
       <c r="E211" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="1" t="n"/>
+      <c r="A212" s="1" t="n">
+        <v>6665789.927697444</v>
+      </c>
       <c r="B212" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C212" s="2" t="n">
         <v>42005</v>
@@ -3681,13 +3679,13 @@
         <v>0</v>
       </c>
       <c r="E212" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n"/>
       <c r="B213" s="1" t="n">
-        <v>36.75</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C213" s="2" t="n">
         <v>42005</v>
@@ -3696,13 +3694,13 @@
         <v>0</v>
       </c>
       <c r="E213" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n"/>
       <c r="B214" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C214" s="2" t="n">
         <v>42005</v>
@@ -3711,13 +3709,13 @@
         <v>0</v>
       </c>
       <c r="E214" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n"/>
       <c r="B215" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C215" s="2" t="n">
         <v>42005</v>
@@ -3726,13 +3724,13 @@
         <v>0</v>
       </c>
       <c r="E215" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n"/>
       <c r="B216" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C216" s="2" t="n">
         <v>42005</v>
@@ -3741,13 +3739,13 @@
         <v>0</v>
       </c>
       <c r="E216" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n"/>
       <c r="B217" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C217" s="2" t="n">
         <v>42005</v>
@@ -3756,13 +3754,13 @@
         <v>0</v>
       </c>
       <c r="E217" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n"/>
       <c r="B218" s="1" t="n">
-        <v>36.25</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C218" s="2" t="n">
         <v>42005</v>
@@ -3777,7 +3775,7 @@
     <row r="219">
       <c r="A219" s="1" t="n"/>
       <c r="B219" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C219" s="2" t="n">
         <v>42005</v>
@@ -3786,13 +3784,13 @@
         <v>0</v>
       </c>
       <c r="E219" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n"/>
       <c r="B220" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C220" s="2" t="n">
         <v>42005</v>
@@ -3801,13 +3799,13 @@
         <v>0</v>
       </c>
       <c r="E220" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n"/>
       <c r="B221" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4337833.761519236</v>
       </c>
       <c r="C221" s="2" t="n">
         <v>42005</v>
@@ -3822,7 +3820,7 @@
     <row r="222">
       <c r="A222" s="1" t="n"/>
       <c r="B222" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4325705.254645599</v>
       </c>
       <c r="C222" s="2" t="n">
         <v>42005</v>
@@ -3831,15 +3829,13 @@
         <v>0</v>
       </c>
       <c r="E222" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>60.04999923706055</v>
-      </c>
+      <c r="A223" s="1" t="n"/>
       <c r="B223" s="1" t="n">
-        <v>37.04999923706055</v>
+        <v>4313576.747771963</v>
       </c>
       <c r="C223" s="2" t="n">
         <v>42005</v>
@@ -3848,13 +3844,13 @@
         <v>0</v>
       </c>
       <c r="E223" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n"/>
       <c r="B224" s="1" t="n">
-        <v>36.95000076293945</v>
+        <v>4301448.240898326</v>
       </c>
       <c r="C224" s="2" t="n">
         <v>42005</v>
@@ -3863,13 +3859,13 @@
         <v>0</v>
       </c>
       <c r="E224" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n"/>
       <c r="B225" s="1" t="n">
-        <v>36.84999847412109</v>
+        <v>4289319.734024689</v>
       </c>
       <c r="C225" s="2" t="n">
         <v>42005</v>
@@ -3878,13 +3874,13 @@
         <v>0</v>
       </c>
       <c r="E225" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n"/>
       <c r="B226" s="1" t="n">
-        <v>36.75</v>
+        <v>4277191.227151052</v>
       </c>
       <c r="C226" s="2" t="n">
         <v>42005</v>
@@ -3897,9 +3893,11 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="1" t="n"/>
+      <c r="A227" s="1" t="n">
+        <v>6677918.434571081</v>
+      </c>
       <c r="B227" s="1" t="n">
-        <v>36.65000152587891</v>
+        <v>4446990.323381967</v>
       </c>
       <c r="C227" s="2" t="n">
         <v>42005</v>
@@ -3914,7 +3912,7 @@
     <row r="228">
       <c r="A228" s="1" t="n"/>
       <c r="B228" s="1" t="n">
-        <v>36.54999923706055</v>
+        <v>4434861.81650833</v>
       </c>
       <c r="C228" s="2" t="n">
         <v>42005</v>
@@ -3923,13 +3921,13 @@
         <v>0</v>
       </c>
       <c r="E228" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n"/>
       <c r="B229" s="1" t="n">
-        <v>36.45000076293945</v>
+        <v>4422733.309634693</v>
       </c>
       <c r="C229" s="2" t="n">
         <v>42005</v>
@@ -3944,7 +3942,7 @@
     <row r="230">
       <c r="A230" s="1" t="n"/>
       <c r="B230" s="1" t="n">
-        <v>36.34999847412109</v>
+        <v>4410604.802761056</v>
       </c>
       <c r="C230" s="2" t="n">
         <v>42005</v>
@@ -3953,13 +3951,13 @@
         <v>0</v>
       </c>
       <c r="E230" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n"/>
       <c r="B231" s="1" t="n">
-        <v>36.25</v>
+        <v>4398476.29588742</v>
       </c>
       <c r="C231" s="2" t="n">
         <v>42005</v>
@@ -3974,7 +3972,7 @@
     <row r="232">
       <c r="A232" s="1" t="n"/>
       <c r="B232" s="1" t="n">
-        <v>36.15000152587891</v>
+        <v>4386347.789013783</v>
       </c>
       <c r="C232" s="2" t="n">
         <v>42005</v>
@@ -3983,13 +3981,13 @@
         <v>0</v>
       </c>
       <c r="E232" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n"/>
       <c r="B233" s="1" t="n">
-        <v>36.04999923706055</v>
+        <v>4374219.282140146</v>
       </c>
       <c r="C233" s="2" t="n">
         <v>42005</v>
@@ -4004,7 +4002,7 @@
     <row r="234">
       <c r="A234" s="1" t="n"/>
       <c r="B234" s="1" t="n">
-        <v>35.95000076293945</v>
+        <v>4362090.77526651</v>
       </c>
       <c r="C234" s="2" t="n">
         <v>42005</v>
@@ -4019,7 +4017,7 @@
     <row r="235">
       <c r="A235" s="1" t="n"/>
       <c r="B235" s="1" t="n">
-        <v>35.84999847412109</v>
+        <v>4349962.268392873</v>
       </c>
       <c r="C235" s="2" t="n">
         <v>42005</v>
@@ -4028,29 +4026,345 @@
         <v>0</v>
       </c>
       <c r="E235" t="n">
-        <v>75</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n"/>
+      <c r="B236" s="1" t="n">
+        <v>4337833.761519236</v>
+      </c>
+      <c r="C236" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D236" t="n">
+        <v>0</v>
+      </c>
+      <c r="E236" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n"/>
+      <c r="B237" s="1" t="n">
+        <v>4325705.254645599</v>
+      </c>
+      <c r="C237" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D237" t="n">
+        <v>0</v>
+      </c>
+      <c r="E237" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n"/>
+      <c r="B238" s="1" t="n">
+        <v>4313576.747771963</v>
+      </c>
+      <c r="C238" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D238" t="n">
+        <v>0</v>
+      </c>
+      <c r="E238" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n"/>
+      <c r="B239" s="1" t="n">
+        <v>4301448.240898326</v>
+      </c>
+      <c r="C239" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D239" t="n">
+        <v>0</v>
+      </c>
+      <c r="E239" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n"/>
+      <c r="B240" s="1" t="n">
+        <v>4289319.734024689</v>
+      </c>
+      <c r="C240" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D240" t="n">
+        <v>0</v>
+      </c>
+      <c r="E240" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n"/>
+      <c r="B241" s="1" t="n">
+        <v>4277191.227151052</v>
+      </c>
+      <c r="C241" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D241" t="n">
+        <v>0</v>
+      </c>
+      <c r="E241" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>6690046.941444717</v>
+      </c>
+      <c r="B242" s="1" t="n">
+        <v>4446990.323381967</v>
+      </c>
+      <c r="C242" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D242" t="n">
+        <v>0</v>
+      </c>
+      <c r="E242" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n"/>
+      <c r="B243" s="1" t="n">
+        <v>4434861.81650833</v>
+      </c>
+      <c r="C243" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D243" t="n">
+        <v>0</v>
+      </c>
+      <c r="E243" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n"/>
+      <c r="B244" s="1" t="n">
+        <v>4422733.309634693</v>
+      </c>
+      <c r="C244" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D244" t="n">
+        <v>0</v>
+      </c>
+      <c r="E244" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n"/>
+      <c r="B245" s="1" t="n">
+        <v>4410604.802761056</v>
+      </c>
+      <c r="C245" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D245" t="n">
+        <v>0</v>
+      </c>
+      <c r="E245" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n"/>
+      <c r="B246" s="1" t="n">
+        <v>4398476.29588742</v>
+      </c>
+      <c r="C246" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D246" t="n">
+        <v>0</v>
+      </c>
+      <c r="E246" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n"/>
+      <c r="B247" s="1" t="n">
+        <v>4386347.789013783</v>
+      </c>
+      <c r="C247" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D247" t="n">
+        <v>0</v>
+      </c>
+      <c r="E247" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n"/>
+      <c r="B248" s="1" t="n">
+        <v>4374219.282140146</v>
+      </c>
+      <c r="C248" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D248" t="n">
+        <v>0</v>
+      </c>
+      <c r="E248" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n"/>
+      <c r="B249" s="1" t="n">
+        <v>4362090.77526651</v>
+      </c>
+      <c r="C249" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D249" t="n">
+        <v>0</v>
+      </c>
+      <c r="E249" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n"/>
+      <c r="B250" s="1" t="n">
+        <v>4349962.268392873</v>
+      </c>
+      <c r="C250" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D250" t="n">
+        <v>0</v>
+      </c>
+      <c r="E250" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n"/>
+      <c r="B251" s="1" t="n">
+        <v>4337833.761519236</v>
+      </c>
+      <c r="C251" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D251" t="n">
+        <v>0</v>
+      </c>
+      <c r="E251" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n"/>
+      <c r="B252" s="1" t="n">
+        <v>4325705.254645599</v>
+      </c>
+      <c r="C252" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D252" t="n">
+        <v>0</v>
+      </c>
+      <c r="E252" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n"/>
+      <c r="B253" s="1" t="n">
+        <v>4313576.747771963</v>
+      </c>
+      <c r="C253" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D253" t="n">
+        <v>0</v>
+      </c>
+      <c r="E253" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n"/>
+      <c r="B254" s="1" t="n">
+        <v>4301448.240898326</v>
+      </c>
+      <c r="C254" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D254" t="n">
+        <v>0</v>
+      </c>
+      <c r="E254" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n"/>
+      <c r="B255" s="1" t="n">
+        <v>4289319.734024689</v>
+      </c>
+      <c r="C255" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D255" t="n">
+        <v>0</v>
+      </c>
+      <c r="E255" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n"/>
+      <c r="B256" s="1" t="n">
+        <v>4277191.227151052</v>
+      </c>
+      <c r="C256" s="2" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D256" t="n">
+        <v>0</v>
+      </c>
+      <c r="E256" t="n">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A15:A27"/>
-    <mergeCell ref="A28:A40"/>
-    <mergeCell ref="A41:A53"/>
-    <mergeCell ref="A54:A66"/>
-    <mergeCell ref="A67:A79"/>
-    <mergeCell ref="A80:A92"/>
-    <mergeCell ref="A93:A105"/>
-    <mergeCell ref="A106:A118"/>
-    <mergeCell ref="A119:A131"/>
-    <mergeCell ref="A132:A144"/>
-    <mergeCell ref="A145:A157"/>
-    <mergeCell ref="A158:A170"/>
-    <mergeCell ref="A171:A183"/>
-    <mergeCell ref="A184:A196"/>
-    <mergeCell ref="A197:A209"/>
-    <mergeCell ref="A210:A222"/>
-    <mergeCell ref="A223:A235"/>
+  <mergeCells count="17">
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A31"/>
+    <mergeCell ref="A32:A46"/>
+    <mergeCell ref="A47:A61"/>
+    <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A77:A91"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
+    <mergeCell ref="A167:A181"/>
+    <mergeCell ref="A182:A196"/>
+    <mergeCell ref="A197:A211"/>
+    <mergeCell ref="A212:A226"/>
+    <mergeCell ref="A227:A241"/>
+    <mergeCell ref="A242:A256"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>